<commit_message>
New version of CYRS after check CYRS_Review Signed-off-by: Donia102950 <donia1995mohamed@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/CYRS_Review.xlsx
+++ b/Input Documents/CYRS_Review.xlsx
@@ -562,12 +562,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,33 +609,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -946,7 +946,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -967,206 +967,189 @@
   <sheetData>
     <row r="2" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="40"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="25">
+      <c r="C7" s="26"/>
+      <c r="D7" s="31">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="36"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1183,6 +1166,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1484,7 +1484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1501,7 +1501,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1512,7 +1512,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1523,7 +1523,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1534,7 +1534,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1545,7 +1545,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1556,7 +1556,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1567,7 +1567,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1578,7 +1578,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1589,7 +1589,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1600,7 +1600,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1611,7 +1611,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1622,7 +1622,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1633,7 +1633,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1644,7 +1644,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>

</xml_diff>

<commit_message>
Modification to the CYRS_Review Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/CYRS_Review.xlsx
+++ b/Input Documents/CYRS_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A21A54B-DCD1-4CAB-A7B8-3D7D17E6FE8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -194,7 +195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -614,8 +615,8 @@
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -946,14 +947,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1112,7 +1113,7 @@
       <c r="G14" s="31"/>
       <c r="H14" s="32"/>
     </row>
-    <row r="15" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -1121,7 +1122,7 @@
       <c r="G15" s="31"/>
       <c r="H15" s="32"/>
     </row>
-    <row r="16" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -1130,7 +1131,7 @@
       <c r="G16" s="31"/>
       <c r="H16" s="32"/>
     </row>
-    <row r="17" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -1139,7 +1140,7 @@
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
     </row>
-    <row r="18" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="36"/>
       <c r="D18" s="36"/>
@@ -1190,11 +1191,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,9 +1259,7 @@
       <c r="F2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
         <v>23</v>
       </c>
@@ -1285,9 +1284,7 @@
       <c r="F3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
@@ -1315,9 +1312,7 @@
       <c r="F4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
         <v>23</v>
       </c>
@@ -1345,9 +1340,7 @@
       <c r="F5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
         <v>23</v>
       </c>
@@ -1372,9 +1365,7 @@
       <c r="F6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
         <v>23</v>
       </c>
@@ -1402,9 +1393,7 @@
       <c r="F7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
         <v>23</v>
       </c>
@@ -1413,7 +1402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>30</v>
       </c>
@@ -1432,9 +1421,7 @@
       <c r="F8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G8" s="10"/>
       <c r="H8" s="10" t="s">
         <v>23</v>
       </c>
@@ -1459,9 +1446,7 @@
       <c r="F9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="G9" s="10"/>
       <c r="H9" s="10" t="s">
         <v>23</v>
       </c>
@@ -1907,10 +1892,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$3:$K$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$6:$K$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/CYRS_Review.xlsx
+++ b/Input Documents/CYRS_Review.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A21A54B-DCD1-4CAB-A7B8-3D7D17E6FE8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE8C6CD-0726-41DA-8ABE-1A55C4D05EE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,12 +563,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,36 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -968,189 +968,206 @@
   <sheetData>
     <row r="2" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="30"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="31">
+      <c r="C7" s="33"/>
+      <c r="D7" s="25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="35"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1167,23 +1184,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1195,7 +1195,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>